<commit_message>
Add PCRSimulatorV4 based on new code
</commit_message>
<xml_diff>
--- a/Examples.xlsx
+++ b/Examples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guorlei/Documents/berkeley/sp20/bioe140l/independent_proj/pcr-plugin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE0C1FA-BEB4-F24E-B0F7-EB1D21AE0E4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F052E248-819B-184B-AF62-873E2F48D06D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{0499FB3D-CA90-F149-B3BF-63D904153723}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>TCCCTGCAAGACGGTGAGTTCATCTACAAAGTTAAACTGCGTGGTACCAACTTCCCGTCCGACGGTCCGGTTATGCAGAAAAAAACCATGGGTTGGGAAGCTTCCACCGAACGTATGTACCCGGAAGACGGTGCTCTGAAAGGTGAAATCAAAATGCGTCTGAAACTGAAAGACGGTGGTCACTACGACGCTGAAGTTAAAACCACCTACATGGCTAAAAAACCGGTTCAGCTGCCGGGTGCTTACAAAACCGACATCAAACTGGACATCACCTCCCACAACGAAGACTACACCATCGTTGAACAGTACGAACGTGCTGAAGGTCGTCACTCCACCGGTGCTTAATAAGGATCTCCAGGCATCAAATAAAACGAAAGGCTCAGTCGAAAGACTGGGCCTTTCGTTTTATCTGTTGTTTGTCGGTGAACGCTCTCTACTAGAGTCACACTGGCTCACCTTCGGGTGGGCCTTTCTGCGTTTATAGGATCCtaaCTCGAcgtgcaggcttcctcgctcactgactcgctgcgctcggtcgttcggctgcggcgagcggtatcagctcactcaaaggcggtaatCAATTCGACCCAGCTTTCTTGTACAAAGTTGGCATTATAAAAAATAATTGCTCATCAATTTGTTGCAACGAACAGGTCACTATCAGTCAAAATAAAATCATTATTTGCCATCCAGCTGATATCCCCTATAGTGAGTCGTATTACATGGTCATAGCTGTTTCCTGGCAGCTCTGGCCCGTGTCTCAAAATCTCTGATGTTACATTGCACAAGATAAAAATATATCATCATGCCTCCTCTAGACCAGCCAGGACAGAAATGCCTCGACTTCGCTGCTGCCCAAGGTTGCCGGGTGACGCACACCGTGGAAACGGATGAAGGCACGAACCCAGTGGACATAAGCCTGTTCGGTTCGTAAGCTGTAATGCAAGTAGCGTATGCGCTCACGCAACTGGTCCAGAACCTTGACCGAACGCAGCGGTGGTAACGGCGCAGTGGCGGTTTTCATGGCTTGTTATGACTGTTTTTTTGGGGTACAGTCTATGCCTCGGGCATCCAAGCAGCAAGCGCGTTACGCCGTGGGTCGATGTTTGATGTTATGGAGCAGCAACGATGTTACGCAGCAGGGCAGTCGCCCTAAAACAAAGTTAAACATCATGAGGGAAGCGGTGATCGCCGAAGTATCGACTCAACTATCAGAGGTAGTTGGCGTCATCGAGCGCCATCTCGAACCGACGTTGCTGGCCGTACATTTGTACGGCTCCGCAGTGGATGGCGGCCTGAAGCCACACAGTGATATTGATTTGCTGGTTACGGTGACCGTAAGGCTTGATGAAACAACGCGGCGAGCTTTGATCAACGACCTTTTGGAAACTTCGGCTTCCCCTGGAGAGAGCGAGATTCTCCGCGCTGTAGAAGTCACCATTGTTGTGCACGACGACATCATTCCGTGGCGTTATCCAGCTAAGCGCGAACTGCAATTTGGAGAATGGCAGCGCAATGACATTCTTGCAGGTATCTTCGAGCCAGCCACGATCGACATTGATCTGGCTATCTTGCTGACAAAAGCAAGAGAACATAGCGTTGCCTTGGTAGGTCCAGCGGCGGAGGAACTCTTTGATCCGGTTCCTGAACAGGATCTATTTGAGGCGCTAAATGAAACCTTAACGCTATGGAACTCGCCGCCCGACTGGGCTGGCGATGAGCGAAATGTAGTGCTTACGTTGTCCCGCATTTGGTACAGCGCAGTAACCGGCAAAATCGCGCCGAAGGATGTCGCTGCCGACTGGGCAATGGAGCGCCTGCCGGCCCAGTATCAGCCCGTCATACTTGAAGCTAGACAGGCTTATCTTGGACAAGAAGAAGATCGCTTGGCCTCGCGCGCAGATCAGTTGGAAGAATTTGTCCACTACGTGAAAGGCGAGATCACCAAGGTAGTCGGCAAATAACCCTCGAGCCACCCATGACCAAAATCCCTTAACGTGAGTTACGCGTCGTTCCACTGAGCGTCAGACCCCGTAGAAAAGATCAAAGGATCTTCTTGAGATCCTTTTTTTCTGCGCGTAATCTGCTGCTTGCAAACAAAAAAACCACCGCTACCAGCGGTGGTTTGTTTGCCGGATCAAGAGCTACCAACTCTTTTTCCGAAGGTAACTGGCTTCAGCAGAGCGCAGATACCAAATACTGTCCTTCTAGTGTAGCCGTAGTTAGGCCACCACTTCAAGAACTCTGTAGCACCGCCTACATACCTCGCTCTGCTAATCCTGTTACCAGTGGCTGCTGCCAGTGGCGATAAGTCGTGTCTTACCGGGTTGGACTCAAGACGATAGTTACCGGATAAGGCGCAGCGGTCGGGCTGAACGGGGGGTTCGTGCACACAGCCCAGCTTGGAGCGAACGACCTACACCGAACTGAGATACCTACAGCGTGAGCATTGAGAAAGCGCCACGCTTCCCGAAGGGAGAAAGGCGGACAGGTATCCGGTAAGCGGCAGGGTCGGAACAGGAGAGCGCACGAGGGAGCTTCCAGGGGGAAACGCCTGGTATCTTTATAGTCCTGTCGGGTTTCGCCACCTCTGACTTGAGCGTCGATTTTTGTGATGCTCGTCAGGGGGGCGGAGCCTATGGAAAAACGCCAGCAACGCGGCCTTTTTACGGTTCCTGGCCTTTTGCTGGCCTTTTGCTCACATGTTCTTTCCTGCGTTATCCCCTGATTCTGTGGATAACCGTcctaggTGTAAAACGACGGCCAGTCTTAAGCTCGGGCCCCAAATAATGATTTTATTTTGACTGATAGTGACCTGTTCGTTGCAACAAATTGATGAGCAATGCTTTTTTATAATGCCAACTTTGTACAAAAAAGCAGGCTCCGAATTGgtatcacgaggcagaatttcagataaaaaaaatccttagctttcgctaaggatgatttctgGAATTCATGAGATCTTCCCTATCAGTGATAGAGATTGACATCCCTATCAGTGATAGAGATACTGAGCACGGATCTGAAAGAGGAGAAAGGATCTATGGCAAGTAGCGAAGACGTTATCAAAGAGTTCATGCGTTTCAAAGTTCGTATGGAAGGTTCCGTTAACGGTCACGAGTTCGAAATCGAAGGTGAAGGTGAAGGTCGTCCGTACGAAGGTACCCAGACCGCTAAACTGAAAGTTACCAAAGGTGGTCCGCTGCCGTTCGCTTGGGACATCCTGTCCCCGCAGTTCCAGTACGGTTCCAAAGCTTACGTTAAACACCCGGCTGACATCCCGGACTACCTGAAACTGTCCTTCCCGGAAGGTTTCAAATGGGAACGTGTTATGAACTTCGAAGACGGTGGTGTTGTTACCGTTACCCAGGACTCC</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>PCR_V3</t>
+  </si>
+  <si>
+    <t>PCR_V4</t>
   </si>
 </sst>
 </file>
@@ -227,6 +230,7 @@
       <definedName name="PCR_v1"/>
       <definedName name="PCR_V2"/>
       <definedName name="PCR_V3"/>
+      <definedName name="PCR_V4"/>
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -533,10 +537,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB01833-FBA1-8941-8EED-812B146F9DBD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -545,10 +549,11 @@
     <col min="2" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="42.83203125" customWidth="1"/>
     <col min="6" max="6" width="44.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="48.83203125" customWidth="1"/>
+    <col min="8" max="8" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
+    <row r="1" spans="1:8" ht="17">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -570,8 +575,11 @@
       <c r="G1" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="17">
+    <row r="2" spans="1:8" ht="17">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -596,8 +604,12 @@
         <f t="array" ref="G2">[1]!PCR_V3(B2,C2,D2)</f>
         <v>CCAGTGAATTCGTCCTCTAGAGAGCTGATCCTTCAACTCAGCAAAAGTTCGATTTATTCAACAAAGCCACGTTGTGTCTCAAAATCTCTGATGTTACATTGCACAAGATAAAAATATATCATCATGAACAATAAAACTGTCTGCTTACATAAACAGTAATACAAGGGGTGTTATGAGCCATATTCAACGGGAAACGTCTTGCTCCAGGCCGCGATTAAATTCCAACATGGATGCTGATTTATATGGGTATAAATGGGCTCGCGATAATGTCGGGCAATCAGGTGCGACAATCTATCGATTGTATGGGAAGCCCGATGCGCCAGAGTTGTTTCTGAAACATGGCAAAGGTAGCGTTGCCAATGATGTTACAGATGAGATGGTCAGACTAAACTGGCTGACGGAATTTATGCCTCTTCCGACCATCAAGCATTTTATCCGTACTCCTGATGATGCATGGTTACTCACCACTGCGATCCCCGGGAAAACAGCATTCCAGGTATTAGAAGAATATCCTGATTCAGGTGAAAATATTGTTGATGCGCTGGCAGTGTTCCTGCGCCGGTTGCATTCGATTCCTGTTTGTAATTGTCCTTTTAACAGCGATCGCGTATTTCGTCTCGCTCAGGCGCAATCACGAATGAATAACGGTTTGGTTGATGCGAGTGATTTTGATGACGAGCGTAATGGCTGGCCTGTTGAACAAGTCTGGAAAGAAATGCATAAGCTTTTGCCATTCTCACCGGATTCAGTCGTCACTCATGGTGATTTCTCACTTGATAACCTTATTTTTGACGAGGGGAAATTAATAGGTTGTATTGATGTTGGACGAGTCGGAATCGCAGACCGATACCAGGATCTTGCCATCCTATGGAACTGCCTCGGTGAGTTTTCTCCTTCATTACAGAAACGGCTTTTTCAAAAATATGGTATTGATAATCCTGATATGAATAAATTGCAGTTTCATTTGATGCTCGATGAGTTTTTCTAATCAGAATTGGTTAATTGGTTGTAACACTGGCAGAGCATTACGCTGACTTGACGGAACTAGTACTGC</v>
       </c>
+      <c r="H2" t="str" cm="1">
+        <f t="array" ref="H2">[1]!PCR_V4(B2,C2,D2)</f>
+        <v>CCAGTGAATTCGTCCTCTAGAGAGCTGATCCTTCAACTCAGCAAAAGTTCGATTTATTCAACAAAGCCACGTTGTGTCTCAAAATCTCTGATGTTACATTGCACAAGATAAAAATATATCATCATGAACAATAAAACTGTCTGCTTACATAAACAGTAATACAAGGGGTGTTATGAGCCATATTCAACGGGAAACGTCTTGCTCCAGGCCGCGATTAAATTCCAACATGGATGCTGATTTATATGGGTATAAATGGGCTCGCGATAATGTCGGGCAATCAGGTGCGACAATCTATCGATTGTATGGGAAGCCCGATGCGCCAGAGTTGTTTCTGAAACATGGCAAAGGTAGCGTTGCCAATGATGTTACAGATGAGATGGTCAGACTAAACTGGCTGACGGAATTTATGCCTCTTCCGACCATCAAGCATTTTATCCGTACTCCTGATGATGCATGGTTACTCACCACTGCGATCCCCGGGAAAACAGCATTCCAGGTATTAGAAGAATATCCTGATTCAGGTGAAAATATTGTTGATGCGCTGGCAGTGTTCCTGCGCCGGTTGCATTCGATTCCTGTTTGTAATTGTCCTTTTAACAGCGATCGCGTATTTCGTCTCGCTCAGGCGCAATCACGAATGAATAACGGTTTGGTTGATGCGAGTGATTTTGATGACGAGCGTAATGGCTGGCCTGTTGAACAAGTCTGGAAAGAAATGCATAAGCTTTTGCCATTCTCACCGGATTCAGTCGTCACTCATGGTGATTTCTCACTTGATAACCTTATTTTTGACGAGGGGAAATTAATAGGTTGTATTGATGTTGGACGAGTCGGAATCGCAGACCGATACCAGGATCTTGCCATCCTATGGAACTGCCTCGGTGAGTTTTCTCCTTCATTACAGAAACGGCTTTTTCAAAAATATGGTATTGATAATCCTGATATGAATAAATTGCAGTTTCATTTGATGCTCGATGAGTTTTTCTAATCAGAATTGGTTAATTGGTTGTAACACTGGCAGAGCATTACGCTGACTTGACGGAACTAGTACTGC</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="17">
+    <row r="3" spans="1:8" ht="17">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -622,8 +634,12 @@
         <f t="array" ref="G3">[1]!PCR_V3(B3,C3,D3)</f>
         <v>CCAAAAGATCTATGAGCGGCTTCCCCCGCAGCGTCGTCGTCGGCGGCAGCGGGGCGGTGGGCGGCATGTTCGCCGGGCTGCTGCGGGAGGCGGGCAGCCGCACGCTCGTCGTCGACCTCGTACCGCCGCCGGGACGGCCGGACGCCTGCCTGGTGGGCGACGTCACCGCGCCGGGGCCCGAACTCGCGGCCGCCCTCCGGGACGCGGACCTCGTCCTGCTCGCCGTACACGAGGACGTGGCCCTCAAGGCCGTGGCGCCCGTGACCCGGCTCATGCGGCCGGGCGCGCTGCTCGCCGACACCCTGTCCGTCCGGACGGGCATGGCCGCGGAGCTCGCGGCCCACGCCCCCGGCGTCCAGCACGTGGGCCTCAACCCGATGTTCGCCCCCGCCGCCGGCATGACCGGCCGACCCGTGGCCGCCGTGGTCACCAGGGACGGGCCGGGCGTCACGGCCCTGCTGCGGCTCGTCGAGGGCGGCGGCGGCAGGCCCGTACGGCTCACGGCGGAGGAGCACGACCGGACGACGGCGGCCACCCAGGCCCTGACGCACGCCGTGCTCCTCTCCTTCGGGCTCGCCCTCGCCCGCCTCGGCGTCGACGTCCGGGCCCTGGCGGCGACGGCACCGCCGCCCCACCAGGTGCTGCTCGCCCTCCTGGCCCGTGTGCTCGGCGGCAGCCCCGAGGTGTACGGGGACATCCAGCGGTCCAACCCCCGGGCGGCGTCCGCGCGCCGGGCGCTCGCCGAGGCCCTGCGCTCCTTCGCCGCGCTGGTCGGCGACGACCCGGACCGTGCCGACGCCCCCGGGCGCGCCGACGCCCCCGGCCATCCCGGGGGATGCGACGGCGCCGGGAACCTCGACGGCGTCTTCGGGGAACTCCGCCGGCTCATGGGACCGGAGCTCGCGGCGGGCCAGGACCACTGCCAGGAGCTGTTCCGCACCCTCCACCGCACCGACGACGAAGGCGAGAAGGACCGATGAGGATCCTAACTCGAGCTAGC</v>
       </c>
+      <c r="H3" t="str" cm="1">
+        <f t="array" ref="H3">[1]!PCR_V4(B3,C3,D3)</f>
+        <v>CCAAAAGATCTATGAGCGGCTTCCCCCGCAGCGTCGTCGTCGGCGGCAGCGGGGCGGTGGGCGGCATGTTCGCCGGGCTGCTGCGGGAGGCGGGCAGCCGCACGCTCGTCGTCGACCTCGTACCGCCGCCGGGACGGCCGGACGCCTGCCTGGTGGGCGACGTCACCGCGCCGGGGCCCGAACTCGCGGCCGCCCTCCGGGACGCGGACCTCGTCCTGCTCGCCGTACACGAGGACGTGGCCCTCAAGGCCGTGGCGCCCGTGACCCGGCTCATGCGGCCGGGCGCGCTGCTCGCCGACACCCTGTCCGTCCGGACGGGCATGGCCGCGGAGCTCGCGGCCCACGCCCCCGGCGTCCAGCACGTGGGCCTCAACCCGATGTTCGCCCCCGCCGCCGGCATGACCGGCCGACCCGTGGCCGCCGTGGTCACCAGGGACGGGCCGGGCGTCACGGCCCTGCTGCGGCTCGTCGAGGGCGGCGGCGGCAGGCCCGTACGGCTCACGGCGGAGGAGCACGACCGGACGACGGCGGCCACCCAGGCCCTGACGCACGCCGTGCTCCTCTCCTTCGGGCTCGCCCTCGCCCGCCTCGGCGTCGACGTCCGGGCCCTGGCGGCGACGGCACCGCCGCCCCACCAGGTGCTGCTCGCCCTCCTGGCCCGTGTGCTCGGCGGCAGCCCCGAGGTGTACGGGGACATCCAGCGGTCCAACCCCCGGGCGGCGTCCGCGCGCCGGGCGCTCGCCGAGGCCCTGCGCTCCTTCGCCGCGCTGGTCGGCGACGACCCGGACCGTGCCGACGCCCCCGGGCGCGCCGACGCCCCCGGCCATCCCGGGGGATGCGACGGCGCCGGGAACCTCGACGGCGTCTTCGGGGAACTCCGCCGGCTCATGGGACCGGAGCTCGCGGCGGGCCAGGACCACTGCCAGGAGCTGTTCCGCACCCTCCACCGCACCGACGACGAAGGCGAGAAGGACCGATGAGGATCCTAACTCGAGCTAGC</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="17">
+    <row r="4" spans="1:8" ht="17">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -648,8 +664,12 @@
         <f t="array" ref="G4">[1]!PCR_V3(B4,C4,"")</f>
         <v>CCATAGAATTCGGAGAGATGCCGGAGCGGCTGAACGGACCGGTNNNNNNNNACCGGAGTAGGGGCAACTCTACCGGGGGTTCAAATCCCCCTCTCTCCGCCACTGCAGATGAC</v>
       </c>
+      <c r="H4" t="str" cm="1">
+        <f t="array" ref="H4">[1]!PCR_V4(B4,C4,"")</f>
+        <v>CCATAGAATTCGGAGAGATGCCGGAGCGGCTGAACGGACCGGTNNNNNNNNACCGGAGTAGGGGCAACTCTACCGGGGGTTCAAATCCCCCTCTCTCCGCCACTGCAGATGAC</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="17">
+    <row r="5" spans="1:8" ht="17">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -674,8 +694,12 @@
         <f t="array" ref="G5">[1]!PCR_V3(B5,C5,D5)</f>
         <v>No PCR product generated.</v>
       </c>
+      <c r="H5" t="str" cm="1">
+        <f t="array" ref="H5">[1]!PCR_V4(B5,C5,D5)</f>
+        <v>CCATAACTAGTCATCGCCGCAGCGGTTTCAGGTTTTAGAGCTAGAAATAGCAAGTTAAAATAAGGCTAGTCCGTTATCAACTTGAAAAAGTGGCACCGAGTCGGTGCTTTTTTTGAATTCTCTAGAGTCGACCTGCAGAAGCTTAGATCTATTACCCTGTTATCCCTACTCGAGTTCATGTGCAGCTCCATAAGCAAAAGGGGATGATAAGTTTATCACCACCGACTATTTGCAACAGTGCCGTTGATCGTGCTATGATCGACTGATGTCATCAGCGGTGGAGTGCAATGTCATGAGGGAAGCGGTGATCGCCGAAGTATCGACTCAACTATCAGAGGTAGTTGGCGTCATCGAGCGCCATCTCGAACCGACGTTGCTGGCCGTACATTTGTACGGCTCCGCAGTGGATGGCGGCCTGAAGCCACACAGTGATATTGATTTGCTGGTTACGGTGACCGTAAGGCTTGATGAAACAACGCGGCGAGCTTTGATCAACGACCTTTTGGAAACTTCGGCTTCCCCTGGAGAGAGCGAGATTCTCCGCGCTGTAGAAGTCACCATTGTTGTGCACGACGACATCATTCCGTGGCGTTATCCAGCTAAGCGCGAACTGCAATTTGGAGAATGGCAGCGCAATGACATTCTTGCAGGTATCTTCGAGCCAGCCACGATCGACATTGATCTGGCTATCTTGCTGACAAAAGCAAGAGAACATAGCGTTGCCTTGGTAGGTCCAGCGGCGGAGGAACTCTTTGATCCGGTTCCTGAACAGGATCTATTTGAGGCGCTAAATGAAACCTTAACGCTATGGAACTCGCCGCCCGACTGGGCTGGCGATGAGCGAAATGTAGTGCTTACGTTGTCCCGCATTTGGTACAGCGCAGTAACCGGCAAAATCGCGCCGAAGGATGTCGCTGCCGACTGGGCAATGGAGCGCCTGCCGGCCCAGTATCAGCCCGTCATACTTGAAGCTAGACAGGCTTATCTTGGACAAGAAGAAGATCGCTTGGCCTCGCGCGCAGATCAGTTGGAAGAATTTGTCCACTACGTGAAAGGCGAGATCACCAAGGTAGTCGGCAAATAAGATGCCGCTCGCCAGTCGATTGGCTGAGCTCATAAGTTCCTATTCCGAAGTTCCGCGAACGCGTAAAGGATCTAGGTGAAGATCCTTTTTGATAATCTCATGACCAAAATCCCTTAACGTGAGTTTTCGTTCCACTGAGCGTCAGACCCCGTAGAAAAGATCAAAGGATCTTCTTGAGATCCTTTTTTTCTGCGCGTAATCTGCTGCTTGCAAACAAAAAAACCACCGCTACCAGCGGTGGTTTGTTTGCCGGATCAAGAGCTACCAACTCTTTTTCCGAAGGTAACTGGCTTCAGCAGAGCGCAGATACCAAATACTGTCCTTCTAGTGTAGCCGTAGTTAGGCCACCACTTCAAGAACTCTGTAGCACCGCCTACATACCTCGCTCTGCTAATCCTGTTACCAGTGGCTGCTGCCAGTGGCGATAAGTCGTGTCTTACCGGGTTGGACTCAAGACGATAGTTACCGGATAAGGCGCAGCGGTCGGGCTGAACGGGGGGTTCGTGCACACAGCCCAGCTTGGAGCGAACGACCTACACCGAACTGAGATACCTACAGCGTGAGCTATGAGAAAGCGCCACGCTTCCCGAAGGGAGAAAGGCGGACAGGTATCCGGTAAGCGGCAGGGTCGGAACAGGAGAGCGCACGAGGGAGCTTCCAGGGGGAAACGCCTGGTATCTTTATAGTCCTGTCGGGTTTCGCCACCTCTGACTTGAGCGTCGATTTTTGTGATGCTCGTCAGGGGGGCGGAGCCTATGGAAAAACGCCAGCAACGCGGCCTTTTTACGGTTCCTGGCCTTTTGCTGGCCTTTTGCTCACATGTTCTTTCCTGCGTTATCCCCTGATTCTGTGGATAACCGTATTACCGCCTTTGAGTGAGCTGATACCGCTCGCCGCAGCCGAACGACCGAGCGCAGCGAGTCAGTGAGCGAGGAAGCGGAAGAGCGCCTGATGCGGTATTTTCTCCTTACGCATCTGTGCGGTATTTCACACCGCATATGCTGGATCCTTGACAGCTAGCTCAGTCCTAGGTATAATACTAGTCTGAG</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="17">
+    <row r="6" spans="1:8" ht="17">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -700,8 +724,12 @@
         <f t="array" ref="G6">[1]!PCR_V3(B6,C6,D6)</f>
         <v>No PCR product generated.</v>
       </c>
+      <c r="H6" t="str" cm="1">
+        <f t="array" ref="H6">[1]!PCR_V4(B6,C6,D6)</f>
+        <v>No PCR product generated.</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" ht="68">
+    <row r="7" spans="1:8" ht="68">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -726,8 +754,12 @@
         <f t="array" ref="G7">[1]!PCR_V3(B7,C7,D7)</f>
         <v>CCAGTGAATTCGTCCTCTAGAGAGCTGATCCTTCAACTCAGCAAAAGTTCGATTTATTCAACAAAGCCACGTTGTGTCTCAAAATCTCTGATGTTACATTGCACAAGATAAAAATATATCATCATGAACAATAAAACTGTCTGCTTACATAAACAGTAATACAAGGGGTGTTATGAGCCATATTCAACGGGAAACGTCTTGCTCCAGGCCGCGATTAAATTCCAACATGGATGCTGATTTATATGGGTATAAATGGGCTCGCGATAATGTCGGGCAATCAGGTGCGACAATCTATCGATTGTATGGGAAGCCCGATGCGCCAGAGTTGTTTCTGAAACATGGCAAAGGTAGCGTTGCCAATGATGTTACAGATGAGATGGTCAGACTAAACTGGCTGACGGAATTTATGCCTCTTCCGACCATCAAGCATTTTATCCGTACTCCTGATGATGCATGGTTACTCACCACTGCGATCCCCGGGAAAACAGCATTCCAGGTATTAGAAGAATATCCTGATTCAGGTGAAAATATTGTTGATGCGCTGGCAGTGTTCCTGCGCCGGTTGCATTCGATTCCTGTTTGTAATTGTCCTTTTAACAGCGATCGCGTATTTCGTCTCGCTCAGGCGCAATCACGAATGAATAACGGTTTGGTTGATGCGAGTGATTTTGATGACGAGCGTAATGGCTGGCCTGTTGAACAAGTCTGGAAAGAAATGCATAAGCTTTTGCCATTCTCACCGGATTCAGTCGTCACTCATGGTGATTTCTCACTTGATAACCTTATTTTTGACGAGGGGAAATTAATAGGTTGTATTGATGTTGGACGAGTCGGAATCGCAGACCGATACCAGGATCTTGCCATCCTATGGAACTGCCTCGGTGAGTTTTCTCCTTCATTACAGAAACGGCTTTTTCAAAAATATGGTATTGATAATCCTGATATGAATAAATTGCAGTTTCATTTGATGCTCGATGAGTTTTTCTAATCAGAATTGGTTAATTGGTTGTAACACTGGCAGAGCATTACGCTGACTTGACGGAACTAGTACTGC</v>
       </c>
+      <c r="H7" t="str" cm="1">
+        <f t="array" ref="H7">[1]!PCR_V4(B7,C7,D7)</f>
+        <v>CCAGTGAATTCGTCCTCTAGAGAGCTGATCCTTCAACTCAGCAAAAGTTCGATTTATTCAACAAAGCCACGTTGTGTCTCAAAATCTCTGATGTTACATTGCACAAGATAAAAATATATCATCATGAACAATAAAACTGTCTGCTTACATAAACAGTAATACAAGGGGTGTTATGAGCCATATTCAACGGGAAACGTCTTGCTCCAGGCCGCGATTAAATTCCAACATGGATGCTGATTTATATGGGTATAAATGGGCTCGCGATAATGTCGGGCAATCAGGTGCGACAATCTATCGATTGTATGGGAAGCCCGATGCGCCAGAGTTGTTTCTGAAACATGGCAAAGGTAGCGTTGCCAATGATGTTACAGATGAGATGGTCAGACTAAACTGGCTGACGGAATTTATGCCTCTTCCGACCATCAAGCATTTTATCCGTACTCCTGATGATGCATGGTTACTCACCACTGCGATCCCCGGGAAAACAGCATTCCAGGTATTAGAAGAATATCCTGATTCAGGTGAAAATATTGTTGATGCGCTGGCAGTGTTCCTGCGCCGGTTGCATTCGATTCCTGTTTGTAATTGTCCTTTTAACAGCGATCGCGTATTTCGTCTCGCTCAGGCGCAATCACGAATGAATAACGGTTTGGTTGATGCGAGTGATTTTGATGACGAGCGTAATGGCTGGCCTGTTGAACAAGTCTGGAAAGAAATGCATAAGCTTTTGCCATTCTCACCGGATTCAGTCGTCACTCATGGTGATTTCTCACTTGATAACCTTATTTTTGACGAGGGGAAATTAATAGGTTGTATTGATGTTGGACGAGTCGGAATCGCAGACCGATACCAGGATCTTGCCATCCTATGGAACTGCCTCGGTGAGTTTTCTCCTTCATTACAGAAACGGCTTTTTCAAAAATATGGTATTGATAATCCTGATATGAATAAATTGCAGTTTCATTTGATGCTCGATGAGTTTTTCTAATCAGAATTGGTTAATTGGTTGTAACACTGGCAGAGCATTACGCTGACTTGACGGAACTAGTACTGC</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" ht="34">
+    <row r="8" spans="1:8" ht="34">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -750,6 +782,10 @@
       </c>
       <c r="G8" t="str" cm="1">
         <f t="array" ref="G8">[1]!PCR_V3(B8,C8,D8)</f>
+        <v>CCAGTGAATTCGTCCTCTAGAGAGCTGATCCTTCAACTCAGCAAAAGTTCGATTTATTCAACAAAGCCACGTTGTGTCTCAAAATCTCTGATGTTACATTGCACAAGATAAAAATATATCATCATGAACAATAAAACTGTCTGCTTACATAAACAGTAATACAAGGGGTGTTATGAGCCATATTCAACGGGAAACGTCTTGCTCCAGGCCGCGATTAAATTCCAACATGGATGCTGATTTATATGGGTATAAATGGGCTCGCGATAATGTCGGGCAATCAGGTGCGACAATCTATCGATTGTATGGGAAGCCCGATGCGCCAGAGTTGTTTCTGAAACATGGCAAAGGTAGCGTTGCCAATGATGTTACAGATGAGATGGTCAGACTAAACTGGCTGACGGAATTTATGCCTCTTCCGACCATCAAGCATTTTATCCGTACTCCTGATGATGCATGGTTACTCACCACTGCGATCCCCGGGAAAACAGCATTCCAGGTATTAGAAGAATATCCTGATTCAGGTGAAAATATTGTTGATGCGCTGGCAGTGTTCCTGCGCCGGTTGCATTCGATTCCTGTTTGTAATTGTCCTTTTAACAGCGATCGCGTATTTCGTCTCGCTCAGGCGCAATCACGAATGAATAACGGTTTGGTTGATGCGAGTGATTTTGATGACGAGCGTAATGGCTGGCCTGTTGAACAAGTCTGGAAAGAAATGCATAAGCTTTTGCCATTCTCACCGGATTCAGTCGTCACTCATGGTGATTTCTCACTTGATAACCTTATTTTTGACGAGGGGAAATTAATAGGTTGTATTGATGTTGGACGAGTCGGAATCGCAGACCGATACCAGGATCTTGCCATCCTATGGAACTGCCTCGGTGAGTTTTCTCCTTCATTACAGAAACGGCTTTTTCAAAAATATGGTATTGATAATCCTGATATGAATAAATTGCAGTTTCATTTGATGCTCGATGAGTTTTTCTAATCAGAATTGGTTAATTGGTTGTAACACTGGCAGAGCATTACGCTGACTTGACGGAACTAGTACTGC</v>
+      </c>
+      <c r="H8" t="str" cm="1">
+        <f t="array" ref="H8">[1]!PCR_V4(B8,C8,D8)</f>
         <v>CCAGTGAATTCGTCCTCTAGAGAGCTGATCCTTCAACTCAGCAAAAGTTCGATTTATTCAACAAAGCCACGTTGTGTCTCAAAATCTCTGATGTTACATTGCACAAGATAAAAATATATCATCATGAACAATAAAACTGTCTGCTTACATAAACAGTAATACAAGGGGTGTTATGAGCCATATTCAACGGGAAACGTCTTGCTCCAGGCCGCGATTAAATTCCAACATGGATGCTGATTTATATGGGTATAAATGGGCTCGCGATAATGTCGGGCAATCAGGTGCGACAATCTATCGATTGTATGGGAAGCCCGATGCGCCAGAGTTGTTTCTGAAACATGGCAAAGGTAGCGTTGCCAATGATGTTACAGATGAGATGGTCAGACTAAACTGGCTGACGGAATTTATGCCTCTTCCGACCATCAAGCATTTTATCCGTACTCCTGATGATGCATGGTTACTCACCACTGCGATCCCCGGGAAAACAGCATTCCAGGTATTAGAAGAATATCCTGATTCAGGTGAAAATATTGTTGATGCGCTGGCAGTGTTCCTGCGCCGGTTGCATTCGATTCCTGTTTGTAATTGTCCTTTTAACAGCGATCGCGTATTTCGTCTCGCTCAGGCGCAATCACGAATGAATAACGGTTTGGTTGATGCGAGTGATTTTGATGACGAGCGTAATGGCTGGCCTGTTGAACAAGTCTGGAAAGAAATGCATAAGCTTTTGCCATTCTCACCGGATTCAGTCGTCACTCATGGTGATTTCTCACTTGATAACCTTATTTTTGACGAGGGGAAATTAATAGGTTGTATTGATGTTGGACGAGTCGGAATCGCAGACCGATACCAGGATCTTGCCATCCTATGGAACTGCCTCGGTGAGTTTTCTCCTTCATTACAGAAACGGCTTTTTCAAAAATATGGTATTGATAATCCTGATATGAATAAATTGCAGTTTCATTTGATGCTCGATGAGTTTTTCTAATCAGAATTGGTTAATTGGTTGTAACACTGGCAGAGCATTACGCTGACTTGACGGAACTAGTACTGC</v>
       </c>
     </row>

</xml_diff>